<commit_message>
changed total to subtotal
</commit_message>
<xml_diff>
--- a/excelFile1.xlsx
+++ b/excelFile1.xlsx
@@ -39,7 +39,7 @@
     <t>WATER</t>
   </si>
   <si>
-    <t>TOTAL</t>
+    <t>SUBTOTAL</t>
   </si>
 </sst>
 </file>
@@ -382,10 +382,13 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>